<commit_message>
changes to folder structure
</commit_message>
<xml_diff>
--- a/QALD9-Plus-data-preparation/unmapped_entities_output_checked.xlsx
+++ b/QALD9-Plus-data-preparation/unmapped_entities_output_checked.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Master Thesis\LC-QuAD-Query-Test\LC-QuAD-2.0-Query-Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Master Thesis\SPARQL-Query-Translation-QALD9\QALD9-Plus-data-preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05F9245-C909-4840-972E-F1DD447F62C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4861A889-7D48-435D-9537-2AE46755E407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="460">
   <si>
     <t>question_id</t>
   </si>
@@ -1481,7 +1481,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4301,5 +4301,6 @@
     <hyperlink ref="D78" r:id="rId10" xr:uid="{5BCCFEAE-9E19-416E-A4F6-05C51DCF0AD8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>